<commit_message>
p3 cleanup, p4 done
</commit_message>
<xml_diff>
--- a/PHX2/part3/output2.xlsx
+++ b/PHX2/part3/output2.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Part 2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Top AL and NL Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Year WAR Ranking" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF55"/>
+  <dimension ref="A1:AF44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4855,419 +4856,116 @@
       </c>
       <c r="AF44" t="inlineStr"/>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr"/>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
-      <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
-      <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
-      <c r="V45" t="inlineStr"/>
-      <c r="W45" t="inlineStr"/>
-      <c r="X45" t="inlineStr"/>
-      <c r="Y45" t="inlineStr"/>
-      <c r="Z45" t="inlineStr"/>
-      <c r="AA45" t="inlineStr"/>
-      <c r="AB45" t="inlineStr"/>
-      <c r="AC45" t="inlineStr"/>
-      <c r="AD45" t="inlineStr"/>
-      <c r="AE45" t="inlineStr"/>
-      <c r="AF45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr"/>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="n">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>WAR/pos</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B2" t="n">
         <v>595.8</v>
       </c>
-      <c r="E46" t="n">
-        <v>2011</v>
-      </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
-      <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
-      <c r="S46" t="inlineStr"/>
-      <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
-      <c r="W46" t="inlineStr"/>
-      <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr"/>
-      <c r="Z46" t="inlineStr"/>
-      <c r="AA46" t="inlineStr"/>
-      <c r="AB46" t="inlineStr"/>
-      <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr"/>
-      <c r="AE46" t="inlineStr"/>
-      <c r="AF46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr"/>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B3" t="n">
         <v>595.3</v>
       </c>
-      <c r="E47" t="n">
-        <v>2012</v>
-      </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
-      <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
-      <c r="S47" t="inlineStr"/>
-      <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
-      <c r="V47" t="inlineStr"/>
-      <c r="W47" t="inlineStr"/>
-      <c r="X47" t="inlineStr"/>
-      <c r="Y47" t="inlineStr"/>
-      <c r="Z47" t="inlineStr"/>
-      <c r="AA47" t="inlineStr"/>
-      <c r="AB47" t="inlineStr"/>
-      <c r="AC47" t="inlineStr"/>
-      <c r="AD47" t="inlineStr"/>
-      <c r="AE47" t="inlineStr"/>
-      <c r="AF47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B4" t="n">
         <v>594.8</v>
       </c>
-      <c r="E48" t="n">
-        <v>2009</v>
-      </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
-      <c r="S48" t="inlineStr"/>
-      <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
-      <c r="V48" t="inlineStr"/>
-      <c r="W48" t="inlineStr"/>
-      <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
-      <c r="AA48" t="inlineStr"/>
-      <c r="AB48" t="inlineStr"/>
-      <c r="AC48" t="inlineStr"/>
-      <c r="AD48" t="inlineStr"/>
-      <c r="AE48" t="inlineStr"/>
-      <c r="AF48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr"/>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="n">
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B5" t="n">
         <v>594</v>
       </c>
-      <c r="E49" t="n">
-        <v>2010</v>
-      </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
-      <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr"/>
-      <c r="S49" t="inlineStr"/>
-      <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr"/>
-      <c r="V49" t="inlineStr"/>
-      <c r="W49" t="inlineStr"/>
-      <c r="X49" t="inlineStr"/>
-      <c r="Y49" t="inlineStr"/>
-      <c r="Z49" t="inlineStr"/>
-      <c r="AA49" t="inlineStr"/>
-      <c r="AB49" t="inlineStr"/>
-      <c r="AC49" t="inlineStr"/>
-      <c r="AD49" t="inlineStr"/>
-      <c r="AE49" t="inlineStr"/>
-      <c r="AF49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr"/>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="n">
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B6" t="n">
         <v>593.6</v>
       </c>
-      <c r="E50" t="n">
-        <v>2007</v>
-      </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
-      <c r="S50" t="inlineStr"/>
-      <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr"/>
-      <c r="W50" t="inlineStr"/>
-      <c r="X50" t="inlineStr"/>
-      <c r="Y50" t="inlineStr"/>
-      <c r="Z50" t="inlineStr"/>
-      <c r="AA50" t="inlineStr"/>
-      <c r="AB50" t="inlineStr"/>
-      <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr"/>
-      <c r="AE50" t="inlineStr"/>
-      <c r="AF50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr"/>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="n">
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B7" t="n">
         <v>593</v>
       </c>
-      <c r="E51" t="n">
-        <v>2008</v>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr"/>
-      <c r="S51" t="inlineStr"/>
-      <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
-      <c r="W51" t="inlineStr"/>
-      <c r="X51" t="inlineStr"/>
-      <c r="Y51" t="inlineStr"/>
-      <c r="Z51" t="inlineStr"/>
-      <c r="AA51" t="inlineStr"/>
-      <c r="AB51" t="inlineStr"/>
-      <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr"/>
-      <c r="AE51" t="inlineStr"/>
-      <c r="AF51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="n">
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B8" t="n">
         <v>592.8</v>
       </c>
-      <c r="E52" t="n">
-        <v>2015</v>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
-      <c r="S52" t="inlineStr"/>
-      <c r="T52" t="inlineStr"/>
-      <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr"/>
-      <c r="W52" t="inlineStr"/>
-      <c r="X52" t="inlineStr"/>
-      <c r="Y52" t="inlineStr"/>
-      <c r="Z52" t="inlineStr"/>
-      <c r="AA52" t="inlineStr"/>
-      <c r="AB52" t="inlineStr"/>
-      <c r="AC52" t="inlineStr"/>
-      <c r="AD52" t="inlineStr"/>
-      <c r="AE52" t="inlineStr"/>
-      <c r="AF52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="n">
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B9" t="n">
         <v>592</v>
       </c>
-      <c r="E53" t="n">
-        <v>2013</v>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
-      <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
-      <c r="V53" t="inlineStr"/>
-      <c r="W53" t="inlineStr"/>
-      <c r="X53" t="inlineStr"/>
-      <c r="Y53" t="inlineStr"/>
-      <c r="Z53" t="inlineStr"/>
-      <c r="AA53" t="inlineStr"/>
-      <c r="AB53" t="inlineStr"/>
-      <c r="AC53" t="inlineStr"/>
-      <c r="AD53" t="inlineStr"/>
-      <c r="AE53" t="inlineStr"/>
-      <c r="AF53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="n">
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B10" t="n">
         <v>591.6</v>
       </c>
-      <c r="E54" t="n">
-        <v>2016</v>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
-      <c r="S54" t="inlineStr"/>
-      <c r="T54" t="inlineStr"/>
-      <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr"/>
-      <c r="W54" t="inlineStr"/>
-      <c r="X54" t="inlineStr"/>
-      <c r="Y54" t="inlineStr"/>
-      <c r="Z54" t="inlineStr"/>
-      <c r="AA54" t="inlineStr"/>
-      <c r="AB54" t="inlineStr"/>
-      <c r="AC54" t="inlineStr"/>
-      <c r="AD54" t="inlineStr"/>
-      <c r="AE54" t="inlineStr"/>
-      <c r="AF54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="n">
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B11" t="n">
         <v>590.6</v>
       </c>
-      <c r="E55" t="n">
-        <v>2014</v>
-      </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
-      <c r="S55" t="inlineStr"/>
-      <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr"/>
-      <c r="V55" t="inlineStr"/>
-      <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr"/>
-      <c r="Y55" t="inlineStr"/>
-      <c r="Z55" t="inlineStr"/>
-      <c r="AA55" t="inlineStr"/>
-      <c r="AB55" t="inlineStr"/>
-      <c r="AC55" t="inlineStr"/>
-      <c r="AD55" t="inlineStr"/>
-      <c r="AE55" t="inlineStr"/>
-      <c r="AF55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>